<commit_message>
maps now recognize stations on one direction or two directions
</commit_message>
<xml_diff>
--- a/U1.xlsx
+++ b/U1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19440" windowHeight="12840" tabRatio="917" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="19440" windowHeight="12840" tabRatio="917" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="U1 to Harcourt MF" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="24">
   <si>
     <t xml:space="preserve">Service No </t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Service Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OXFORD High Street Carfax </t>
   </si>
   <si>
     <t xml:space="preserve">Frideswide Square R9 </t>
@@ -2853,7 +2850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
@@ -3725,8 +3722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4054,7 +4051,7 @@
     </row>
     <row r="7" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B7" s="75">
         <v>825</v>
@@ -4213,7 +4210,7 @@
     </row>
     <row r="10" spans="1:17" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="75">
         <v>837</v>
@@ -4326,13 +4323,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
@@ -4547,7 +4544,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="78" t="s">
         <v>15</v>
       </c>
@@ -13353,13 +13350,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed reminder swiping feature
</commit_message>
<xml_diff>
--- a/U1.xlsx
+++ b/U1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="19440" windowHeight="12840" tabRatio="917" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="45220" windowHeight="17720" tabRatio="917" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="U1 to Harcourt MF" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,12 @@
     <sheet name="summer U1 harcourt Sun" sheetId="11" r:id="rId11"/>
     <sheet name="summer U1 wheatley Sun" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -96,7 +101,24 @@
     <t>Service Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Frideswide Square R9 </t>
+    <r>
+      <t>Frideswide S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>q</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> R9 </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -183,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -424,6 +446,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -729,17 +754,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR11"/>
   <sheetViews>
-    <sheetView topLeftCell="BE1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BO12" sqref="BO12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="63" max="63" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="63" max="63" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -951,7 +976,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1157,7 +1182,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1353,7 +1378,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:70">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1551,7 +1576,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:70">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1763,7 +1788,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1975,7 +2000,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2187,7 +2212,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:70">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2388,7 +2413,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:70">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2533,7 +2558,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:70">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2687,7 +2712,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:70">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2843,6 +2868,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2854,12 +2884,12 @@
       <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -2951,7 +2981,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" s="39" t="s">
         <v>12</v>
       </c>
@@ -3039,7 +3069,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" s="39" t="s">
         <v>13</v>
       </c>
@@ -3127,7 +3157,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
@@ -3147,7 +3177,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" s="39" t="s">
         <v>21</v>
       </c>
@@ -3167,7 +3197,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" s="39" t="s">
         <v>14</v>
       </c>
@@ -3259,7 +3289,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="27" customHeight="1">
       <c r="A7" s="39" t="s">
         <v>15</v>
       </c>
@@ -3351,7 +3381,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" s="39" t="s">
         <v>6</v>
       </c>
@@ -3443,7 +3473,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" s="39" t="s">
         <v>5</v>
       </c>
@@ -3535,7 +3565,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" s="39" t="s">
         <v>4</v>
       </c>
@@ -3621,7 +3651,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" s="39" t="s">
         <v>3</v>
       </c>
@@ -3715,6 +3745,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3723,15 +3758,15 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
@@ -3784,7 +3819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="74" t="s">
         <v>3</v>
       </c>
@@ -3837,7 +3872,7 @@
         <v>2235</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="74" t="s">
         <v>4</v>
       </c>
@@ -3890,7 +3925,7 @@
         <v>2238</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="74" t="s">
         <v>5</v>
       </c>
@@ -3943,7 +3978,7 @@
         <v>2243</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="74" t="s">
         <v>6</v>
       </c>
@@ -3996,7 +4031,7 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="74" t="s">
         <v>7</v>
       </c>
@@ -4049,7 +4084,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="32.25" customHeight="1">
       <c r="A7" s="74" t="s">
         <v>8</v>
       </c>
@@ -4102,7 +4137,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="74" t="s">
         <v>9</v>
       </c>
@@ -4155,7 +4190,7 @@
         <v>2302</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="74" t="s">
         <v>10</v>
       </c>
@@ -4208,8 +4243,8 @@
         <v>2306</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="39" x14ac:dyDescent="0.25">
-      <c r="A10" s="74" t="s">
+    <row r="10" spans="1:17">
+      <c r="A10" s="81" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="75">
@@ -4261,7 +4296,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="74" t="s">
         <v>12</v>
       </c>
@@ -4316,6 +4351,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4327,12 +4367,12 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
@@ -4385,7 +4425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="78" t="s">
         <v>12</v>
       </c>
@@ -4438,7 +4478,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="78" t="s">
         <v>13</v>
       </c>
@@ -4491,7 +4531,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="78" t="s">
         <v>14</v>
       </c>
@@ -4544,7 +4584,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="26.25" customHeight="1">
       <c r="A5" s="78" t="s">
         <v>15</v>
       </c>
@@ -4597,7 +4637,7 @@
         <v>2315</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="78" t="s">
         <v>6</v>
       </c>
@@ -4650,7 +4690,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" s="78" t="s">
         <v>5</v>
       </c>
@@ -4703,7 +4743,7 @@
         <v>2323</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="78" t="s">
         <v>4</v>
       </c>
@@ -4752,7 +4792,7 @@
         <v>2329</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="78" t="s">
         <v>3</v>
       </c>
@@ -4807,6 +4847,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4814,16 +4859,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT12"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BQ14" sqref="BQ14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:72">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -5041,7 +5086,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:72">
       <c r="A2" s="16" t="s">
         <v>12</v>
       </c>
@@ -5199,7 +5244,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:72">
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
@@ -5357,7 +5402,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:72">
       <c r="A4" s="46" t="s">
         <v>18</v>
       </c>
@@ -5443,7 +5488,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:72">
       <c r="A5" s="64" t="s">
         <v>19</v>
       </c>
@@ -5529,7 +5574,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:72">
       <c r="A6" s="16" t="s">
         <v>14</v>
       </c>
@@ -5739,7 +5784,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:72">
       <c r="A7" s="16" t="s">
         <v>16</v>
       </c>
@@ -5829,7 +5874,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:72" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:72" ht="23.25" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
@@ -6043,7 +6088,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:72">
       <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
@@ -6257,7 +6302,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:72">
       <c r="A10" s="16" t="s">
         <v>5</v>
       </c>
@@ -6467,7 +6512,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:72">
       <c r="A11" s="16" t="s">
         <v>4</v>
       </c>
@@ -6651,7 +6696,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:72">
       <c r="A12" s="16" t="s">
         <v>3</v>
       </c>
@@ -6871,6 +6916,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6882,12 +6932,12 @@
       <selection activeCell="AK20" sqref="AK20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -7003,7 +7053,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38">
       <c r="A2" s="33" t="s">
         <v>3</v>
       </c>
@@ -7119,7 +7169,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38">
       <c r="A3" s="33" t="s">
         <v>4</v>
       </c>
@@ -7235,7 +7285,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38">
       <c r="A4" s="33" t="s">
         <v>5</v>
       </c>
@@ -7351,7 +7401,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38">
       <c r="A5" s="33" t="s">
         <v>6</v>
       </c>
@@ -7467,7 +7517,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38">
       <c r="A6" s="33" t="s">
         <v>7</v>
       </c>
@@ -7583,7 +7633,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" ht="25">
       <c r="A7" s="33" t="s">
         <v>8</v>
       </c>
@@ -7699,7 +7749,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38">
       <c r="A8" s="33" t="s">
         <v>9</v>
       </c>
@@ -7815,7 +7865,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38">
       <c r="A9" s="33" t="s">
         <v>10</v>
       </c>
@@ -7927,7 +7977,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38">
       <c r="A10" s="33" t="s">
         <v>11</v>
       </c>
@@ -8039,7 +8089,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38">
       <c r="A11" s="33" t="s">
         <v>12</v>
       </c>
@@ -8153,6 +8203,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8164,12 +8219,12 @@
       <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -8285,7 +8340,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38">
       <c r="A2" s="39" t="s">
         <v>12</v>
       </c>
@@ -8397,7 +8452,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38">
       <c r="A3" s="39" t="s">
         <v>13</v>
       </c>
@@ -8509,7 +8564,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38">
       <c r="A4" s="39" t="s">
         <v>18</v>
       </c>
@@ -8561,7 +8616,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38">
       <c r="A5" s="39" t="s">
         <v>19</v>
       </c>
@@ -8613,7 +8668,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38">
       <c r="A6" s="39" t="s">
         <v>14</v>
       </c>
@@ -8729,7 +8784,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38">
       <c r="A7" s="39" t="s">
         <v>15</v>
       </c>
@@ -8845,7 +8900,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38">
       <c r="A8" s="39" t="s">
         <v>6</v>
       </c>
@@ -8961,7 +9016,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38">
       <c r="A9" s="39" t="s">
         <v>5</v>
       </c>
@@ -9077,7 +9132,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38">
       <c r="A10" s="39" t="s">
         <v>4</v>
       </c>
@@ -9187,7 +9242,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38">
       <c r="A11" s="39" t="s">
         <v>3</v>
       </c>
@@ -9305,6 +9360,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9316,12 +9376,12 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -9422,7 +9482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33">
       <c r="A2" s="39" t="s">
         <v>3</v>
       </c>
@@ -9523,7 +9583,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33">
       <c r="A3" s="39" t="s">
         <v>4</v>
       </c>
@@ -9624,7 +9684,7 @@
         <v>2338</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33">
       <c r="A4" s="39" t="s">
         <v>5</v>
       </c>
@@ -9725,7 +9785,7 @@
         <v>2343</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33">
       <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
@@ -9826,7 +9886,7 @@
         <v>2349</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33">
       <c r="A6" s="39" t="s">
         <v>7</v>
       </c>
@@ -9927,7 +9987,7 @@
         <v>2354</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="25">
       <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
@@ -10028,7 +10088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33">
       <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
@@ -10129,7 +10189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33">
       <c r="A9" s="39" t="s">
         <v>10</v>
       </c>
@@ -10230,7 +10290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33">
       <c r="A10" s="39" t="s">
         <v>11</v>
       </c>
@@ -10331,7 +10391,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33">
       <c r="A11" s="39" t="s">
         <v>12</v>
       </c>
@@ -10434,6 +10494,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10445,12 +10510,12 @@
       <selection activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -10551,7 +10616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33">
       <c r="A2" s="39" t="s">
         <v>12</v>
       </c>
@@ -10652,7 +10717,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33">
       <c r="A3" s="39" t="s">
         <v>20</v>
       </c>
@@ -10753,7 +10818,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33">
       <c r="A4" s="39" t="s">
         <v>14</v>
       </c>
@@ -10854,7 +10919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33">
       <c r="A5" s="39" t="s">
         <v>15</v>
       </c>
@@ -10955,7 +11020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33">
       <c r="A6" s="39" t="s">
         <v>6</v>
       </c>
@@ -11056,7 +11121,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33">
       <c r="A7" s="39" t="s">
         <v>5</v>
       </c>
@@ -11157,7 +11222,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33">
       <c r="A8" s="39" t="s">
         <v>4</v>
       </c>
@@ -11252,7 +11317,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33">
       <c r="A9" s="39" t="s">
         <v>3</v>
       </c>
@@ -11355,6 +11420,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -11366,12 +11436,12 @@
       <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
@@ -11463,7 +11533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" s="39" t="s">
         <v>3</v>
       </c>
@@ -11553,7 +11623,7 @@
         <v>2235</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" s="39" t="s">
         <v>4</v>
       </c>
@@ -11643,7 +11713,7 @@
         <v>2238</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4" s="39" t="s">
         <v>5</v>
       </c>
@@ -11733,7 +11803,7 @@
         <v>2243</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
@@ -11823,7 +11893,7 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" s="39" t="s">
         <v>7</v>
       </c>
@@ -11915,7 +11985,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
@@ -12007,7 +12077,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
@@ -12099,7 +12169,7 @@
         <v>2302</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" s="39" t="s">
         <v>10</v>
       </c>
@@ -12191,7 +12261,7 @@
         <v>2306</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" s="39" t="s">
         <v>11</v>
       </c>
@@ -12283,7 +12353,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" s="39" t="s">
         <v>12</v>
       </c>
@@ -12377,6 +12447,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -12388,12 +12463,12 @@
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="A1" s="39" t="s">
         <v>22</v>
       </c>
@@ -12497,7 +12572,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34">
       <c r="A2" s="39" t="s">
         <v>12</v>
       </c>
@@ -12593,7 +12668,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34">
       <c r="A3" s="39" t="s">
         <v>13</v>
       </c>
@@ -12689,7 +12764,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34">
       <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
@@ -12713,7 +12788,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34">
       <c r="A5" s="39" t="s">
         <v>21</v>
       </c>
@@ -12737,7 +12812,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34">
       <c r="A6" s="39" t="s">
         <v>14</v>
       </c>
@@ -12839,7 +12914,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34">
       <c r="A7" s="39" t="s">
         <v>15</v>
       </c>
@@ -12941,7 +13016,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34">
       <c r="A8" s="39" t="s">
         <v>6</v>
       </c>
@@ -13043,7 +13118,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34">
       <c r="A9" s="39" t="s">
         <v>5</v>
       </c>
@@ -13147,7 +13222,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10" s="39" t="s">
         <v>4</v>
       </c>
@@ -13237,7 +13312,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11" s="39" t="s">
         <v>3</v>
       </c>
@@ -13343,6 +13418,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -13354,12 +13434,12 @@
       <selection activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -13451,7 +13531,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" s="39" t="s">
         <v>3</v>
       </c>
@@ -13543,7 +13623,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" s="39" t="s">
         <v>4</v>
       </c>
@@ -13635,7 +13715,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4" s="39" t="s">
         <v>5</v>
       </c>
@@ -13727,7 +13807,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
@@ -13819,7 +13899,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" s="39" t="s">
         <v>7</v>
       </c>
@@ -13911,7 +13991,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
@@ -14003,7 +14083,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
@@ -14095,7 +14175,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" s="39" t="s">
         <v>10</v>
       </c>
@@ -14183,7 +14263,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" s="39" t="s">
         <v>11</v>
       </c>
@@ -14271,7 +14351,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" s="39" t="s">
         <v>12</v>
       </c>
@@ -14361,5 +14441,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>